<commit_message>
Fix: bypass total de servidor para descargas
</commit_message>
<xml_diff>
--- a/public/tools/punto-equilibrio.xlsx
+++ b/public/tools/punto-equilibrio.xlsx
@@ -1,160 +1,57 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdrianAlcarazPreciad\Documents\cci-react\public\tools\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73A37A2F-E70C-49B4-B9DA-54E13D941458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Punto de Equilibrio" sheetId="1" r:id="rId1"/>
-    <sheet name="Instrucciones" sheetId="2" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Punto de Equilibrio" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instrucciones" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>CÁLCULO DEL PUNTO DE EQUILIBRIO</t>
-  </si>
-  <si>
-    <t>DATOS DE ENTRADA</t>
-  </si>
-  <si>
-    <t>Precio de Venta Unitario</t>
-  </si>
-  <si>
-    <t>Costo Variable Unitario</t>
-  </si>
-  <si>
-    <t>Costos Fijos Totales</t>
-  </si>
-  <si>
-    <t>RESULTADOS</t>
-  </si>
-  <si>
-    <t>Margen de Contribución Unitario</t>
-  </si>
-  <si>
-    <t>Margen de Contribución (%)</t>
-  </si>
-  <si>
-    <t>Punto de Equilibrio (Unidades)</t>
-  </si>
-  <si>
-    <t>Punto de Equilibrio (Ventas en $)</t>
-  </si>
-  <si>
-    <t>GUÍA PARA USAR LA PLANTILLA – PUNTO DE EQUILIBRIO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-¿QUÉ ES EL PUNTO DE EQUILIBRIO?
-Es la cantidad mínima de unidades que debes vender para cubrir todos tus costos.
-En ese punto no ganas ni pierdes dinero.
-------------------------------------------------------------
-PASO 1: LLENAR LOS DATOS DE ENTRADA (Hoja: Punto de Equilibrio)
-1) Precio de Venta Unitario
-   Es el precio al que vendes tu producto o servicio.
-   Ejemplo: Si vendes una playera en $300, ese es tu precio de venta.
-2) Costo Variable Unitario
-   Es el costo que cambia por cada unidad que produces o vendes.
-   Ejemplo: Tela, comisiones, empaques, envío por producto, etc.
-3) Costos Fijos Totales
-   Son los gastos que pagas aunque no vendas nada.
-   Ejemplo: Renta, sueldos, internet, luz fija, contador, software, etc.
-------------------------------------------------------------
-PASO 2: INTERPRETAR LOS RESULTADOS
-• Margen de Contribución Unitario:
-  Es lo que te queda por cada venta después de pagar el costo variable.
-• Margen de Contribución %:
-  Es el porcentaje de cada venta que ayuda a cubrir tus costos fijos.
-• Punto de Equilibrio (Unidades):
-  Es la cantidad mínima que debes vender para no perder dinero.
-• Punto de Equilibrio (Ventas en $):
-  Es el monto total que necesitas facturar para cubrir todos tus costos.
-------------------------------------------------------------
-RECOMENDACIÓN PRÁCTICA
-Si actualmente vendes menos que el punto de equilibrio:
-   → Estás perdiendo dinero.
-Si vendes exactamente el punto de equilibrio:
-   → No ganas ni pierdes.
-Si vendes más que el punto de equilibrio:
-   → Empiezas a generar utilidad.
-------------------------------------------------------------
-Consejo Empresarial:
-Usa esta herramienta antes de fijar precios o lanzar promociones.
-Nunca bajes precios sin calcular primero tu nuevo punto de equilibrio.
-</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="14"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
       <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF1F4E78"/>
-        <bgColor rgb="FF1F4E78"/>
+        <fgColor rgb="001F4E78"/>
+        <bgColor rgb="001F4E78"/>
       </patternFill>
     </fill>
   </fills>
@@ -167,56 +64,105 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -504,95 +450,116 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
+    <col width="45" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>CÁLCULO DEL PUNTO DE EQUILIBRIO – PERIODO MENSUAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>DATOS DE ENTRADA (MENSUALES)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Precio de Venta Unitario ($ por producto/servicio)</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="9"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2">
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>Costo Variable Unitario ($ por producto/servicio)</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>Costos Fijos Totales Mensuales ($)</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>RESULTADOS (MENSUALES)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="inlineStr">
+        <is>
+          <t>Margen de Contribución Unitario</t>
+        </is>
+      </c>
+      <c r="B9" s="4">
         <f>B4-B5</f>
-        <v>2380</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="4">
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5" t="inlineStr">
+        <is>
+          <t>Margen de Contribución (%)</t>
+        </is>
+      </c>
+      <c r="B10" s="6">
         <f>B9/B4</f>
-        <v>0.95199999999999996</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="5">
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="inlineStr">
+        <is>
+          <t>Punto de Equilibrio (Unidades al Mes)</t>
+        </is>
+      </c>
+      <c r="B11" s="7">
         <f>B6/B9</f>
-        <v>12.605042016806722</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="2">
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t>Punto de Equilibrio (Ventas Mensuales en $)</t>
+        </is>
+      </c>
+      <c r="B12" s="4">
         <f>B11*B4</f>
-        <v>31512.605042016807</v>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -606,26 +573,58 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="110" customWidth="1"/>
+    <col width="110" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>11</v>
+    <row r="1">
+      <c r="A1" s="8" t="inlineStr">
+        <is>
+          <t>GUÍA PARA USAR LA PLANTILLA – PUNTO DE EQUILIBRIO MENSUAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Esta herramienta calcula tu punto de equilibrio considerando un periodo mensual.
+¿QUÉ ES EL PUNTO DE EQUILIBRIO?
+Es la cantidad mínima que debes vender en un mes para cubrir todos tus gastos mensuales.
+En ese punto no ganas ni pierdes dinero.
+------------------------------------------------------------
+PASO 1: LLENAR LOS DATOS (Hoja: Punto de Equilibrio)
+1) Precio de Venta Unitario
+   Precio al que vendes cada producto o servicio.
+2) Costo Variable Unitario
+   Costo que cambia por cada unidad vendida (material, comisión, envío, etc.).
+3) Costos Fijos Totales Mensuales
+   Todos los gastos que pagas cada mes aunque no vendas:
+   renta, sueldos, internet, software, servicios, etc.
+------------------------------------------------------------
+PASO 2: INTERPRETAR RESULTADOS
+• Punto de Equilibrio (Unidades al Mes):
+  Cantidad mínima que debes vender cada mes para no perder dinero.
+• Punto de Equilibrio (Ventas Mensuales en $):
+  Total que necesitas facturar al mes para cubrir tus costos.
+------------------------------------------------------------
+Consejo Empresarial:
+Si tus ventas actuales mensuales están por debajo del punto de equilibrio,
+tu negocio está generando pérdidas.
+</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>